<commit_message>
Working on Excel data load
</commit_message>
<xml_diff>
--- a/newfile25.xlsx
+++ b/newfile25.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="146">
   <si>
     <r>
       <t xml:space="preserve">Образец №1 към чл. 9, ал. 1 на </t>
@@ -59,7 +59,7 @@
     <t>Идентификационен код</t>
   </si>
   <si>
-    <t xml:space="preserve"> Рекуестор Нейм</t>
+    <t>Рекуестор Нейм</t>
   </si>
   <si>
     <t>~</t>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Адрес</t>
+  </si>
+  <si>
+    <t>Рекуестор адрес</t>
   </si>
   <si>
     <r>
@@ -147,6 +150,12 @@
       </rPr>
       <t xml:space="preserve"> Длъжник по обезпеченото вземане и продължение съгласно Приложение №1</t>
     </r>
+  </si>
+  <si>
+    <t>Pledger Name. чакам долна граница 333555777 чакам горна граница oчаквам долна граница АДресчето на пледвера с улица На Баба ти улицата, номер 69, вх. А, ет.6 очаквам горна граница</t>
+  </si>
+  <si>
+    <t>АДресчето на пледвера с улица На Баба ти улицата, номер 69, вх. А, ет.6</t>
   </si>
   <si>
     <r>
@@ -2562,7 +2571,9 @@
       <c r="AJ6" s="15"/>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -2602,7 +2613,7 @@
     <row r="8" ht="2.4" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" ht="12" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -2610,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2630,7 +2641,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="Y10" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z10" s="20"/>
       <c r="AA10" s="8"/>
@@ -2745,7 +2756,7 @@
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2867,8 +2878,10 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="23"/>
     </row>
-    <row r="17" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+    <row r="17" ht="12" customHeight="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -2896,16 +2909,37 @@
       <c r="Z17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA17" s="34"/>
-      <c r="AB17" s="34"/>
-      <c r="AC17" s="34"/>
-      <c r="AD17" s="34"/>
-      <c r="AE17" s="34"/>
-      <c r="AF17" s="34"/>
-      <c r="AG17" s="34"/>
-      <c r="AH17" s="34"/>
-      <c r="AI17" s="34"/>
-      <c r="AJ17" s="34"/>
+      <c r="AA17" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB17" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC17" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD17" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE17" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF17" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG17" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH17" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ17" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK17" s="1"/>
     </row>
     <row r="18" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
@@ -2950,7 +2984,9 @@
       <c r="AJ18" s="9"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="35" t="s">
+        <v>17</v>
+      </c>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
@@ -3027,7 +3063,7 @@
     </row>
     <row r="21" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3150,7 +3186,9 @@
       <c r="AJ23" s="23"/>
     </row>
     <row r="24" ht="12" customHeight="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -3178,16 +3216,36 @@
       <c r="Z24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
-      <c r="AE24" s="12"/>
-      <c r="AF24" s="12"/>
-      <c r="AG24" s="12"/>
-      <c r="AH24" s="12"/>
-      <c r="AI24" s="12"/>
-      <c r="AJ24" s="12"/>
+      <c r="AA24" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ24" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="AK24" s="36"/>
     </row>
     <row r="25" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -3233,7 +3291,9 @@
       <c r="AJ25" s="9"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -3310,7 +3370,7 @@
     </row>
     <row r="28" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3434,7 +3494,7 @@
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -3539,7 +3599,7 @@
     </row>
     <row r="33" ht="14.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -3617,7 +3677,7 @@
     </row>
     <row r="35" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3660,7 +3720,7 @@
         <v>11</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -3680,7 +3740,7 @@
         <v>12</v>
       </c>
       <c r="R36" s="29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S36" s="8"/>
       <c r="T36" s="8"/>
@@ -3696,7 +3756,7 @@
         <v>14</v>
       </c>
       <c r="AD36" s="41" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AE36" s="40"/>
       <c r="AF36" s="39"/>
@@ -3707,7 +3767,7 @@
     </row>
     <row r="37" ht="24" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="42"/>
@@ -3725,7 +3785,7 @@
       <c r="O37" s="42"/>
       <c r="P37" s="42"/>
       <c r="Q37" s="43" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R37" s="43"/>
       <c r="S37" s="43"/>
@@ -3739,7 +3799,7 @@
       <c r="AA37" s="43"/>
       <c r="AB37" s="43"/>
       <c r="AC37" s="44" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AD37" s="44"/>
       <c r="AE37" s="44"/>
@@ -3754,7 +3814,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -3786,7 +3846,7 @@
         <v>15</v>
       </c>
       <c r="AD38" s="41" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AE38" s="41"/>
       <c r="AF38" s="41"/>
@@ -3797,7 +3857,7 @@
     </row>
     <row r="39" ht="21" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="45" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B39" s="45"/>
       <c r="C39" s="45"/>
@@ -3827,7 +3887,7 @@
       <c r="AA39" s="45"/>
       <c r="AB39" s="45"/>
       <c r="AC39" s="44" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="AD39" s="44"/>
       <c r="AE39" s="44"/>
@@ -3877,7 +3937,7 @@
     </row>
     <row r="41" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3920,7 +3980,7 @@
         <v>16</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -3959,7 +4019,7 @@
     </row>
     <row r="43" ht="14.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
@@ -4037,7 +4097,7 @@
     </row>
     <row r="45" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4080,7 +4140,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -4119,7 +4179,7 @@
     </row>
     <row r="47" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B47" s="46"/>
       <c r="C47" s="46"/>
@@ -4352,7 +4412,7 @@
         <v>18</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="47"/>
@@ -4372,7 +4432,7 @@
         <v>19</v>
       </c>
       <c r="R53" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="S53" s="8"/>
       <c r="T53" s="8"/>
@@ -4411,7 +4471,7 @@
       <c r="O54" s="47"/>
       <c r="P54" s="47"/>
       <c r="Q54" s="28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="R54" s="27"/>
       <c r="S54" s="27"/>
@@ -4468,7 +4528,7 @@
     </row>
     <row r="56" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -4506,7 +4566,7 @@
         <v>20</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -4516,7 +4576,7 @@
         <v>21</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="40"/>
@@ -4594,7 +4654,7 @@
       <c r="F59" s="23"/>
       <c r="G59" s="1"/>
       <c r="H59" s="48" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I59" s="48"/>
       <c r="J59" s="48"/>
@@ -4629,7 +4689,7 @@
       <c r="A60" s="28"/>
       <c r="B60" s="38"/>
       <c r="C60" s="27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D60" s="38"/>
       <c r="E60" s="27"/>
@@ -4705,12 +4765,12 @@
     </row>
     <row r="62" ht="12" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -4730,7 +4790,7 @@
       <c r="Q63" s="8"/>
       <c r="R63" s="9"/>
       <c r="S63" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="T63" s="8"/>
       <c r="U63" s="8"/>
@@ -4790,7 +4850,7 @@
     </row>
     <row r="65" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B65" s="52"/>
       <c r="C65" s="52"/>
@@ -4802,7 +4862,7 @@
       <c r="I65" s="52"/>
       <c r="J65" s="52"/>
       <c r="K65" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L65" s="52"/>
       <c r="M65" s="52"/>
@@ -4812,7 +4872,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="23"/>
       <c r="S65" s="51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="T65" s="52"/>
       <c r="U65" s="52"/>
@@ -4824,7 +4884,7 @@
       <c r="AA65" s="52"/>
       <c r="AB65" s="52"/>
       <c r="AC65" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AD65" s="52"/>
       <c r="AE65" s="52"/>
@@ -4912,12 +4972,12 @@
     </row>
     <row r="68" ht="12" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" ht="10.5" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -4939,7 +4999,7 @@
       <c r="S69" s="8"/>
       <c r="T69" s="8"/>
       <c r="U69" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V69" s="54"/>
       <c r="W69" s="54"/>
@@ -4951,7 +5011,7 @@
       <c r="AC69" s="54"/>
       <c r="AD69" s="54"/>
       <c r="AE69" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF69" s="54"/>
       <c r="AG69" s="54"/>
@@ -5142,7 +5202,7 @@
       <c r="AB74" s="1"/>
       <c r="AC74" s="1"/>
       <c r="AD74" s="56" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AE74" s="1"/>
       <c r="AF74" s="1"/>
@@ -5153,13 +5213,13 @@
     </row>
     <row r="75" ht="12" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AB75" s="57"/>
     </row>
     <row r="76" ht="11.25" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -5172,7 +5232,7 @@
       <c r="J76" s="8"/>
       <c r="K76" s="9"/>
       <c r="L76" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M76" s="8"/>
       <c r="N76" s="8"/>
@@ -5187,7 +5247,7 @@
       <c r="W76" s="8"/>
       <c r="X76" s="9"/>
       <c r="Y76" s="58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Z76" s="8"/>
       <c r="AA76" s="8"/>
@@ -5195,7 +5255,7 @@
       <c r="AC76" s="8"/>
       <c r="AD76" s="9"/>
       <c r="AE76" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF76" s="54"/>
       <c r="AG76" s="54"/>
@@ -5251,7 +5311,7 @@
     </row>
     <row r="79" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AE79" s="1"/>
       <c r="AF79" s="1"/>
@@ -5262,7 +5322,7 @@
     </row>
     <row r="80" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -5270,7 +5330,7 @@
       <c r="E80" s="8"/>
       <c r="F80" s="9"/>
       <c r="G80" s="58" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
@@ -5296,7 +5356,7 @@
       <c r="AC80" s="8"/>
       <c r="AD80" s="9"/>
       <c r="AE80" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF80" s="54"/>
       <c r="AG80" s="54"/>
@@ -5345,17 +5405,17 @@
     <row r="82" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="59"/>
       <c r="B82" s="60" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D82" s="54"/>
       <c r="E82" s="54"/>
       <c r="F82" s="54"/>
       <c r="G82" s="55"/>
       <c r="H82" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I82" s="54"/>
       <c r="J82" s="54"/>
@@ -5369,14 +5429,14 @@
       <c r="R82" s="54"/>
       <c r="S82" s="55"/>
       <c r="T82" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="U82" s="54"/>
       <c r="V82" s="54"/>
       <c r="W82" s="54"/>
       <c r="X82" s="55"/>
       <c r="Y82" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Z82" s="54"/>
       <c r="AA82" s="54"/>
@@ -5384,7 +5444,7 @@
       <c r="AC82" s="54"/>
       <c r="AD82" s="55"/>
       <c r="AE82" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF82" s="54"/>
       <c r="AG82" s="54"/>
@@ -5395,7 +5455,7 @@
     <row r="83" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="28"/>
       <c r="B83" s="61" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C83" s="28"/>
       <c r="D83" s="27"/>
@@ -5435,12 +5495,12 @@
     <row r="84" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" ht="12" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -5448,7 +5508,7 @@
       <c r="E86" s="8"/>
       <c r="F86" s="9"/>
       <c r="G86" s="58" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
@@ -5474,7 +5534,7 @@
       <c r="AC86" s="8"/>
       <c r="AD86" s="9"/>
       <c r="AE86" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF86" s="54"/>
       <c r="AG86" s="54"/>
@@ -5523,10 +5583,10 @@
     <row r="88" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="59"/>
       <c r="B88" s="60" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
@@ -5544,7 +5604,7 @@
       <c r="Q88" s="52"/>
       <c r="R88" s="52"/>
       <c r="S88" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="T88" s="18"/>
       <c r="U88" s="54"/>
@@ -5558,7 +5618,7 @@
       <c r="AC88" s="54"/>
       <c r="AD88" s="55"/>
       <c r="AE88" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF88" s="54"/>
       <c r="AG88" s="54"/>
@@ -5569,7 +5629,7 @@
     <row r="89" ht="12" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="28"/>
       <c r="B89" s="61" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C89" s="28"/>
       <c r="D89" s="27"/>
@@ -5614,26 +5674,26 @@
     <row r="95" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="96" ht="12" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="63" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H96" s="27"/>
     </row>
     <row r="97" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" s="59" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
       <c r="G97" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="8"/>
@@ -5659,7 +5719,7 @@
       <c r="AE97" s="8"/>
       <c r="AF97" s="8"/>
       <c r="AG97" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH97" s="8"/>
       <c r="AI97" s="8"/>
@@ -5667,7 +5727,7 @@
     </row>
     <row r="98" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5698,7 +5758,7 @@
       <c r="AB98" s="1"/>
       <c r="AC98" s="1"/>
       <c r="AD98" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AE98" s="1"/>
       <c r="AF98" s="1"/>
@@ -5709,7 +5769,7 @@
     </row>
     <row r="99" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" s="32" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -5749,7 +5809,7 @@
     </row>
     <row r="100" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" s="32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -5783,7 +5843,7 @@
       <c r="AE100" s="1"/>
       <c r="AF100" s="1"/>
       <c r="AG100" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH100" s="1"/>
       <c r="AI100" s="1"/>
@@ -5791,16 +5851,16 @@
     </row>
     <row r="101" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
@@ -5808,7 +5868,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
@@ -5829,10 +5889,10 @@
       <c r="AC101" s="1"/>
       <c r="AD101" s="1"/>
       <c r="AE101" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AF101" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AG101" s="1"/>
       <c r="AH101" s="1"/>
@@ -5841,7 +5901,7 @@
     </row>
     <row r="102" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -5851,7 +5911,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
@@ -5883,7 +5943,7 @@
     </row>
     <row r="103" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103" s="32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -5917,7 +5977,7 @@
       <c r="AE103" s="1"/>
       <c r="AF103" s="1"/>
       <c r="AG103" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AH103" s="1"/>
       <c r="AI103" s="1"/>
@@ -5925,16 +5985,16 @@
     </row>
     <row r="104" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
@@ -5942,7 +6002,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
@@ -5963,10 +6023,10 @@
       <c r="AC104" s="1"/>
       <c r="AD104" s="1"/>
       <c r="AE104" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AF104" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AG104" s="1"/>
       <c r="AH104" s="1"/>
@@ -5975,7 +6035,7 @@
     </row>
     <row r="105" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" s="32" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -5985,7 +6045,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
@@ -6017,12 +6077,12 @@
     </row>
     <row r="106" ht="14.1" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -6047,19 +6107,19 @@
       <c r="Y106" s="1"/>
       <c r="Z106" s="1"/>
       <c r="AA106" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AB106" s="1"/>
       <c r="AC106" s="1"/>
       <c r="AD106" s="1"/>
       <c r="AE106" s="1"/>
       <c r="AF106" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AG106" s="1"/>
       <c r="AH106" s="1"/>
       <c r="AI106" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AJ106" s="23"/>
     </row>
@@ -6117,7 +6177,7 @@
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
@@ -6128,7 +6188,7 @@
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
       <c r="X108" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Y108" s="1"/>
       <c r="Z108" s="1"/>
@@ -6632,7 +6692,7 @@
   <sheetData>
     <row r="1" ht="15.6" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -6672,7 +6732,7 @@
     </row>
     <row r="2" ht="13.8" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -6788,7 +6848,7 @@
     </row>
     <row r="5" ht="15.6" customHeight="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="73" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B5" s="73"/>
       <c r="C5" s="73"/>
@@ -6866,7 +6926,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="75" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" s="72"/>
@@ -7072,7 +7132,7 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="75" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
@@ -7322,7 +7382,7 @@
     <row r="1" ht="13.8" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="72"/>
       <c r="B1" s="90" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="72"/>
@@ -7352,7 +7412,7 @@
       <c r="AB1" s="72"/>
       <c r="AC1" s="72"/>
       <c r="AD1" s="91" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AE1" s="91"/>
       <c r="AF1" s="91"/>
@@ -7464,7 +7524,7 @@
     <row r="4" ht="24.75" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="72"/>
       <c r="B4" s="95" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C4" s="95"/>
       <c r="D4" s="95"/>
@@ -7512,7 +7572,7 @@
     <row r="5" ht="12" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="72"/>
       <c r="B5" s="96" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C5" s="96"/>
       <c r="D5" s="96"/>
@@ -7708,7 +7768,7 @@
     <row r="9" ht="10.5" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="72"/>
       <c r="B9" s="98" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C9" s="79"/>
       <c r="D9" s="79"/>
@@ -7833,7 +7893,7 @@
       <c r="Z11" s="79"/>
       <c r="AA11" s="79"/>
       <c r="AB11" s="105" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AC11" s="79"/>
       <c r="AD11" s="79"/>
@@ -7950,7 +8010,7 @@
     <row r="14" ht="15" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="72"/>
       <c r="B14" s="109" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C14" s="109"/>
       <c r="D14" s="109"/>
@@ -8045,7 +8105,7 @@
       <c r="A16" s="72"/>
       <c r="B16" s="72"/>
       <c r="C16" s="110" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D16" s="72"/>
       <c r="E16" s="72"/>
@@ -8138,7 +8198,7 @@
     <row r="18" ht="12" customHeight="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" s="72"/>
       <c r="B18" s="112" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="72"/>
@@ -8187,7 +8247,7 @@
     <row r="19" ht="11.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
       <c r="B19" s="98" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C19" s="79"/>
       <c r="D19" s="79"/>
@@ -8461,7 +8521,7 @@
     <row r="24" ht="14.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="72"/>
       <c r="B24" s="90" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C24" s="72"/>
       <c r="D24" s="72"/>
@@ -8481,7 +8541,7 @@
       <c r="R24" s="72"/>
       <c r="S24" s="72"/>
       <c r="U24" s="90" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="V24" s="115"/>
       <c r="W24" s="90"/>
@@ -8596,7 +8656,7 @@
       <c r="C27" s="120"/>
       <c r="D27" s="72"/>
       <c r="E27" s="13" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F27" s="72"/>
       <c r="G27" s="72"/>
@@ -8614,21 +8674,21 @@
       <c r="S27" s="72"/>
       <c r="U27" s="122"/>
       <c r="V27" s="123" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="W27" s="72"/>
       <c r="Y27" s="72"/>
       <c r="Z27" s="120" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AB27" s="123" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AE27" s="72"/>
       <c r="AF27" s="72"/>
       <c r="AH27" s="120"/>
       <c r="AI27" s="13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AJ27" s="72"/>
       <c r="AK27" s="124"/>
@@ -8688,11 +8748,11 @@
       <c r="A29" s="72"/>
       <c r="B29" s="119"/>
       <c r="C29" s="120" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D29" s="72"/>
       <c r="E29" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F29" s="72"/>
       <c r="G29" s="72"/>
@@ -8714,7 +8774,7 @@
       <c r="X29" s="76"/>
       <c r="Y29" s="76"/>
       <c r="Z29" s="126" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AA29" s="126"/>
       <c r="AB29" s="126"/>
@@ -8831,7 +8891,7 @@
       <c r="C32" s="120"/>
       <c r="D32" s="72"/>
       <c r="E32" s="13" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F32" s="72"/>
       <c r="G32" s="72"/>
@@ -8848,7 +8908,7 @@
       <c r="R32" s="121"/>
       <c r="S32" s="72"/>
       <c r="U32" s="115" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AA32" s="72"/>
       <c r="AB32" s="72"/>
@@ -8922,7 +8982,7 @@
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
       <c r="E34" s="98" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F34" s="79"/>
       <c r="G34" s="79"/>
@@ -8941,7 +9001,7 @@
       <c r="U34" s="119"/>
       <c r="V34" s="120"/>
       <c r="W34" s="72" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="X34" s="72"/>
       <c r="Y34" s="72"/>
@@ -8954,7 +9014,7 @@
       <c r="AF34" s="72"/>
       <c r="AG34" s="120"/>
       <c r="AH34" s="72" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AI34" s="72"/>
       <c r="AJ34" s="72"/>
@@ -9035,7 +9095,7 @@
       <c r="U36" s="119"/>
       <c r="V36" s="120"/>
       <c r="W36" s="72" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="X36" s="72"/>
       <c r="Y36" s="72"/>
@@ -9048,7 +9108,7 @@
       <c r="AF36" s="72"/>
       <c r="AG36" s="120"/>
       <c r="AH36" s="72" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AI36" s="72"/>
       <c r="AJ36" s="72"/>
@@ -9112,7 +9172,7 @@
       <c r="C38" s="120"/>
       <c r="D38" s="72"/>
       <c r="E38" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F38" s="72"/>
       <c r="G38" s="72"/>
@@ -9131,7 +9191,7 @@
       <c r="U38" s="119"/>
       <c r="V38" s="120"/>
       <c r="W38" s="72" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="X38" s="72"/>
       <c r="Y38" s="72"/>
@@ -9144,7 +9204,7 @@
       <c r="AF38" s="72"/>
       <c r="AG38" s="120"/>
       <c r="AH38" s="72" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AI38" s="72"/>
       <c r="AJ38" s="72"/>
@@ -9208,7 +9268,7 @@
       <c r="C40" s="120"/>
       <c r="D40" s="72"/>
       <c r="E40" s="13" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F40" s="72"/>
       <c r="G40" s="72"/>
@@ -9227,7 +9287,7 @@
       <c r="U40" s="119"/>
       <c r="V40" s="120"/>
       <c r="W40" s="72" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="X40" s="72"/>
       <c r="Y40" s="72"/>
@@ -9240,7 +9300,7 @@
       <c r="AF40" s="72"/>
       <c r="AG40" s="120"/>
       <c r="AH40" s="72" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AI40" s="72"/>
       <c r="AJ40" s="72"/>
@@ -9305,7 +9365,7 @@
       <c r="C42" s="72"/>
       <c r="D42" s="72"/>
       <c r="E42" s="98" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" s="118"/>
       <c r="G42" s="79"/>
@@ -9369,7 +9429,7 @@
       <c r="S43" s="72"/>
       <c r="T43" s="72"/>
       <c r="U43" s="131" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="V43" s="115"/>
       <c r="W43" s="115"/>
@@ -9447,7 +9507,7 @@
       <c r="C45" s="120"/>
       <c r="D45" s="72"/>
       <c r="E45" s="13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F45" s="72"/>
       <c r="G45" s="72"/>
@@ -9466,10 +9526,10 @@
       <c r="T45" s="72"/>
       <c r="U45" s="119"/>
       <c r="V45" s="120" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="W45" s="72" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="X45" s="72"/>
       <c r="Y45" s="72"/>
@@ -9545,7 +9605,7 @@
       <c r="C47" s="72"/>
       <c r="D47" s="72"/>
       <c r="E47" s="98" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F47" s="118"/>
       <c r="G47" s="79"/>
@@ -9564,10 +9624,10 @@
       <c r="T47" s="72"/>
       <c r="U47" s="119"/>
       <c r="V47" s="120" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="W47" s="72" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="X47" s="72"/>
       <c r="Y47" s="72"/>
@@ -9664,7 +9724,7 @@
       <c r="V49" s="133"/>
       <c r="W49" s="134"/>
       <c r="X49" s="135" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="Y49" s="135"/>
       <c r="Z49" s="135"/>
@@ -9802,7 +9862,7 @@
       <c r="R52" s="72"/>
       <c r="S52" s="72"/>
       <c r="V52" s="90" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="W52" s="72"/>
       <c r="X52" s="72"/>
@@ -9921,7 +9981,7 @@
     <row r="55" ht="14.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A55" s="72"/>
       <c r="B55" s="149" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C55" s="76"/>
       <c r="D55" s="76"/>
@@ -10015,7 +10075,7 @@
     <row r="57" ht="22.5" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A57" s="121"/>
       <c r="B57" s="152" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C57" s="152"/>
       <c r="D57" s="152"/>
@@ -10041,7 +10101,7 @@
       <c r="X57" s="152"/>
       <c r="Y57" s="152"/>
       <c r="Z57" s="72" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AA57" s="72"/>
       <c r="AB57" s="153"/>
@@ -10065,7 +10125,7 @@
     <row r="58" ht="9" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A58" s="121"/>
       <c r="B58" s="13" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C58" s="72"/>
       <c r="D58" s="72"/>
@@ -10113,7 +10173,7 @@
     <row r="59" ht="20.25" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A59" s="121"/>
       <c r="B59" s="154" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C59" s="154"/>
       <c r="D59" s="154"/>
@@ -10207,7 +10267,7 @@
     <row r="61" ht="6.75" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A61" s="121"/>
       <c r="B61" s="156" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C61" s="156"/>
       <c r="D61" s="156"/>
@@ -10284,7 +10344,7 @@
       <c r="AC62" s="156"/>
       <c r="AD62" s="156"/>
       <c r="AF62" s="157" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AG62" s="79"/>
       <c r="AH62" s="79"/>
@@ -10393,7 +10453,7 @@
     <row r="65" ht="21.75" customHeight="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A65" s="72"/>
       <c r="B65" s="112" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C65" s="72"/>
       <c r="D65" s="72"/>
@@ -10441,7 +10501,7 @@
     <row r="66" ht="12" customHeight="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A66" s="72"/>
       <c r="B66" s="98" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C66" s="79"/>
       <c r="D66" s="79"/>
@@ -10472,7 +10532,7 @@
       <c r="AC66" s="163"/>
       <c r="AD66" s="163"/>
       <c r="AE66" s="98" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AF66" s="163"/>
       <c r="AG66" s="79"/>

</xml_diff>

<commit_message>
Continue work for Excell Writter
</commit_message>
<xml_diff>
--- a/newfile25.xlsx
+++ b/newfile25.xlsx
@@ -211,7 +211,7 @@
     <t>банков кредит</t>
   </si>
   <si>
-    <t>ПРАЙМ БК"  +  3 , минимум  2</t>
+    <t>ПРАЙМ БК"  +  3 , минимум  2%</t>
   </si>
   <si>
     <t>Размер ( с цифри и думи)</t>
@@ -220,10 +220,10 @@
     <t>Лихви за забава</t>
   </si>
   <si>
-    <t>………………. BGN/EUR /… словом - размер на кредита …./</t>
-  </si>
-  <si>
-    <t>Прайм БК за …… + …%, минимум …%</t>
+    <t>BGN10000 /десет хиляди лева</t>
+  </si>
+  <si>
+    <t>ПРАЙМ БК"  + 13, минимум 12%</t>
   </si>
   <si>
     <r>
@@ -264,7 +264,7 @@
     <t>Описание</t>
   </si>
   <si>
-    <t>Особен залог върху всички настоящи и бъдещи вземания на Залогодателя към Банката за наличностите по банкови сметки с IBAN: BG……….., BG……………., открити при Юробанк България АД, както и по всички открити в последствие сметки в Банката, по които ще постъпят вземания, включително за допълнително постъпили средства по сметките, включително за начислените и изплатени лихви по тях, за сума в размер на BGN/EUR ....размера на кредита... /....словом.../.</t>
+    <t>особен залог на всички настоящи и бъдещи вземания на Залогодателя към Банката за наличностите по банкова сметка: IBAN № BG67ALABALA.., открита при Юробанк България" АД, както и по всички открити в последствие сметки в Банката, по които ще постъпят вземанията, включително за допълнително постъпили средства по сметките, включително за начислените и изплатени лихви по тях, за сума в размер на BGN 50000/ Сметката е открита съгласно договор за разплащателна сметка /по-долу "Договора за сметка"/ от 30/02/2015г</t>
   </si>
   <si>
     <t>Цена</t>

</xml_diff>